<commit_message>
Python (Pyplot + Scipy) Ge 1 assignment and Update of Many Sets
</commit_message>
<xml_diff>
--- a/Ge_1_Sets/Lab3.xlsx
+++ b/Ge_1_Sets/Lab3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Mathematica\Ge_1_Sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2CEEA6-7E2F-4160-9446-05FB0E551229}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B00A633-1328-4CAC-AF5C-6099C647F50A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20604" windowHeight="5700" activeTab="1" xr2:uid="{CCBC6983-18A1-4374-B3D6-9A520B64FE5D}"/>
   </bookViews>
@@ -790,10 +790,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -801,14 +798,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cornstarch</a:t>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Corn Syrup</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> Post-Glacial Rebound Displacement over Time</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -827,10 +836,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1230,10 +1236,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1241,7 +1244,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Time (s)</a:t>
                 </a:r>
               </a:p>
@@ -1262,10 +1269,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1284,10 +1288,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1300,10 +1301,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1333,10 +1331,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1344,7 +1339,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Displacement (mm)</a:t>
                 </a:r>
               </a:p>
@@ -1365,10 +1364,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1387,10 +1383,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1403,10 +1396,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1444,12 +1434,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1495,10 +1480,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1506,11 +1488,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cornstract Post-Glacial Rebound Log</a:t>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Corn Syrup Post-Glacial Rebound Semi-Log Plot</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> of Displacement over time</a:t>
             </a:r>
           </a:p>
@@ -1531,10 +1521,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1934,10 +1921,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1945,7 +1929,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Time (s)</a:t>
                 </a:r>
               </a:p>
@@ -1966,10 +1954,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1988,10 +1973,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2004,10 +1986,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2037,10 +2016,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2048,8 +2024,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Ln(Displacement)</a:t>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Ln(Displacement (mm))</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2069,10 +2049,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2091,10 +2068,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2107,10 +2081,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2148,12 +2119,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2505,10 +2471,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2516,14 +2479,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Post-Glacial Rebound of the Fennoscandian Ice Sheet</a:t>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Semi-Log Post-Glacial Rebound of the Fennoscandian Ice Sheet</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> from 9320 years ago to the present</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2542,10 +2517,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2558,7 +2530,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12254184893554973"/>
+          <c:y val="0.14864197530864198"/>
+          <c:w val="0.84058572308091117"/>
+          <c:h val="0.69387295723836995"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2588,11 +2570,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2602,9 +2588,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -2614,8 +2600,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.5409886264216972E-2"/>
-                  <c:y val="0.337561606882473"/>
+                  <c:x val="3.9182414698162728E-2"/>
+                  <c:y val="0.2348611111111111"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2736,10 +2722,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2747,7 +2730,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Age (Years)</a:t>
                 </a:r>
               </a:p>
@@ -2768,10 +2755,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2790,10 +2774,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2806,10 +2787,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2839,10 +2817,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2850,7 +2825,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Ln(Displacement from Equilibrium (m))</a:t>
                 </a:r>
               </a:p>
@@ -2860,8 +2839,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="3.0555555555555555E-2"/>
-              <c:y val="0.1115277777777778"/>
+              <c:x val="2.6346912723417503E-2"/>
+              <c:y val="0.19751169340991537"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2879,10 +2858,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2901,10 +2877,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2917,10 +2890,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2958,12 +2928,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -5813,9 +5778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>262890</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>10668</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5843,15 +5808,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:colOff>529590</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>128016</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5921,14 +5886,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>41910</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>346710</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>35052</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6255,8 +6220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65504BC4-3627-4F7A-9C76-6523A040046A}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="F24" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7286,8 +7251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29725A1C-F15E-4DE6-85D1-606FBCCB47C6}">
   <dimension ref="A3:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>